<commit_message>
Changed default delimiter character from '~' to '.'. Updated example files accordingly. Fixes #10
</commit_message>
<xml_diff>
--- a/examples/VASP_to_thermdat/example1/references.xlsx
+++ b/examples/VASP_to_thermdat/example1/references.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UDel Documents\UDel Research\Github\PyMuTT\examples\VASP_to_thermdat\example1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0544A5E9-4A6B-42D1-B90C-A6C6EDFFF5EB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4349396F-6A3E-479F-BAFF-CB2FEFAF0EA1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5364" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,12 +102,6 @@
     <t>Stoichiometric formula</t>
   </si>
   <si>
-    <t>elements~H</t>
-  </si>
-  <si>
-    <t>elements~O</t>
-  </si>
-  <si>
     <t>Vibrational wavenumber in 1/cm</t>
   </si>
   <si>
@@ -124,6 +118,12 @@
   </si>
   <si>
     <t>vib_wavenumber</t>
+  </si>
+  <si>
+    <t>elements.H</t>
+  </si>
+  <si>
+    <t>elements.O</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,10 +525,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -555,13 +555,13 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -580,7 +580,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>17</v>
@@ -604,13 +604,13 @@
         <v>23</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3">
         <v>298</v>
@@ -646,7 +646,7 @@
         <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -672,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4">
         <v>298</v>
@@ -688,7 +688,7 @@
         <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K4">
         <v>2</v>

</xml_diff>

<commit_message>
Reworked BaseThermo and Nasa
References issue #15
The attributes T_ref and HoRT_ref were removed from BaseThermo and put into a new class, References.

Split Nasa's __init__ method into 3 methods depending on the inputs.
__init__ is for inputting NASA polynomials directly.
from_data is for fitting the NASA polynomial to Ts, CpoR, T_ref, HoRT_ref, SoR_ref
from_statmech is for fitting the NASA polynomial from a StatMech model
</commit_message>
<xml_diff>
--- a/examples/VASP_to_thermdat/example1/references.xlsx
+++ b/examples/VASP_to_thermdat/example1/references.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UDel Documents\UDel Research\Github\PyMuTT\examples\VASP_to_thermdat\example1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4349396F-6A3E-479F-BAFF-CB2FEFAF0EA1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2390AB34-33E2-4500-9D0A-7AA8A717F835}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5364" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,11 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -33,9 +38,6 @@
     <t>phase</t>
   </si>
   <si>
-    <t>thermo_model</t>
-  </si>
-  <si>
     <t>T_ref</t>
   </si>
   <si>
@@ -124,6 +126,9 @@
   </si>
   <si>
     <t>elements.O</t>
+  </si>
+  <si>
+    <t>statmech_model</t>
   </si>
 </sst>
 </file>
@@ -497,7 +502,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,43 +530,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -570,47 +575,47 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="M2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -619,10 +624,10 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -631,7 +636,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3">
         <v>298</v>
@@ -643,10 +648,10 @@
         <v>-6.7598000000000003</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -660,10 +665,10 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -672,7 +677,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4">
         <v>298</v>
@@ -685,10 +690,10 @@
         <v>-14.2209</v>
       </c>
       <c r="I4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4">
         <v>2</v>

</xml_diff>